<commit_message>
updating excel sheet for testing of encoders
</commit_message>
<xml_diff>
--- a/Electronics/OmoFarouSensorTest/SensorTestSheet.xlsx
+++ b/Electronics/OmoFarouSensorTest/SensorTestSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\myProject\Area_Coverage-DoubleZigZag\Electronics\OmoFarouSensorTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\myProject\CleanerRepo\Area_Coverage\Electronics\OmoFarouSensorTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="2352"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="2352" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Encoder Left" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="39">
   <si>
     <t>#</t>
   </si>
@@ -123,6 +123,52 @@
   </si>
   <si>
     <t>trials #</t>
+  </si>
+  <si>
+    <t>32 turns per 15000 ticks</t>
+  </si>
+  <si>
+    <t>end of line in robot control</t>
+  </si>
+  <si>
+    <t>robot control model in routines subsystem</t>
+  </si>
+  <si>
+    <t>all devices connected except blue and green LEDs and bluetooth</t>
+  </si>
+  <si>
+    <t>motor connected normally in its position and a flag is attached to detect each round</t>
+  </si>
+  <si>
+    <t>give PWM for motor for 15000 ticks, and monitor how many turns it did. Repeat this sequence for different PWMs. 100, 150, 200 and 250</t>
+  </si>
+  <si>
+    <t>matlab model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leftMotorTicksPerCm = 
+or
+leftMotorCmPerTick = </t>
+  </si>
+  <si>
+    <t>PWM</t>
+  </si>
+  <si>
+    <t>number of rounds</t>
+  </si>
+  <si>
+    <t>ticks/round</t>
+  </si>
+  <si>
+    <t>wheelSize (cm)</t>
+  </si>
+  <si>
+    <t>Ticks/Cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rightMotorTicksPerCm = 
+or
+rightMotorCmPerTick = </t>
   </si>
 </sst>
 </file>
@@ -555,12 +601,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.44140625" customWidth="1"/>
     <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.109375" customWidth="1"/>
@@ -569,7 +616,7 @@
     <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.33203125" customWidth="1"/>
     <col min="9" max="9" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -604,29 +651,55 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="B3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -636,11 +709,23 @@
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="B4" s="3">
+        <v>100</v>
+      </c>
+      <c r="C4" s="3">
+        <v>32</v>
+      </c>
+      <c r="D4" s="3">
+        <f>15000/C4</f>
+        <v>468.75</v>
+      </c>
+      <c r="E4" s="3">
+        <v>12</v>
+      </c>
+      <c r="F4" s="3">
+        <f>D4/(2*3.14*(E4/2))</f>
+        <v>12.440286624203821</v>
+      </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -650,11 +735,23 @@
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="B5" s="3">
+        <v>150</v>
+      </c>
+      <c r="C5" s="3">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:D7" si="0">15000/C5</f>
+        <v>468.75</v>
+      </c>
+      <c r="E5" s="3">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" ref="F5:F7" si="1">D5/(2*3.14*(E5/2))</f>
+        <v>12.440286624203821</v>
+      </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -664,11 +761,23 @@
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="B6" s="3">
+        <v>200</v>
+      </c>
+      <c r="C6" s="3">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>468.75</v>
+      </c>
+      <c r="E6" s="3">
+        <v>12</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="1"/>
+        <v>12.440286624203821</v>
+      </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -678,11 +787,23 @@
       <c r="A7" s="13">
         <v>4</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="B7" s="3">
+        <v>250</v>
+      </c>
+      <c r="C7" s="3">
+        <v>32</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>468.75</v>
+      </c>
+      <c r="E7" s="3">
+        <v>12</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="1"/>
+        <v>12.440286624203821</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -710,17 +831,242 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>100</v>
+      </c>
+      <c r="C4" s="3">
+        <v>32</v>
+      </c>
+      <c r="D4" s="3">
+        <f>15000/C4</f>
+        <v>468.75</v>
+      </c>
+      <c r="E4" s="3">
+        <v>12</v>
+      </c>
+      <c r="F4" s="3">
+        <f>D4/(2*3.14*(E4/2))</f>
+        <v>12.440286624203821</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>150</v>
+      </c>
+      <c r="C5" s="3">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:D7" si="0">15000/C5</f>
+        <v>468.75</v>
+      </c>
+      <c r="E5" s="3">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" ref="F5:F7" si="1">D5/(2*3.14*(E5/2))</f>
+        <v>12.440286624203821</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3">
+        <v>200</v>
+      </c>
+      <c r="C6" s="3">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>468.75</v>
+      </c>
+      <c r="E6" s="3">
+        <v>12</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="1"/>
+        <v>12.440286624203821</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="13">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>250</v>
+      </c>
+      <c r="C7" s="3">
+        <v>32</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>468.75</v>
+      </c>
+      <c r="E7" s="3">
+        <v>12</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="1"/>
+        <v>12.440286624203821</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="7"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>